<commit_message>
Update Presupuesto mejoramiento El Sabanal.xlsx
</commit_message>
<xml_diff>
--- a/Infraestructura/Presupuestos/El Sabanal/Presupuesto mejoramiento El Sabanal.xlsx
+++ b/Infraestructura/Presupuestos/El Sabanal/Presupuesto mejoramiento El Sabanal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmadrid/Documents/GitHub/Dotaciones2019/Infraestructura/Presupuestos/El Sabanal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9113C8FC-8E28-B546-8A06-CEB0E29C515F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C38CB9DE-09E6-D443-8F1C-8E8CFE58E7D7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LISTADO DE ITEMS" sheetId="1" r:id="rId1"/>
@@ -2666,7 +2666,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2733,6 +2733,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6600"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -2796,7 +2808,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -2965,10 +2977,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
@@ -3013,6 +3021,27 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="12" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="12" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -3034,10 +3063,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF0000"/>
+      <color rgb="FFFF6600"/>
       <color rgb="FFCC9900"/>
       <color rgb="FFFF5050"/>
-      <color rgb="FFFF6600"/>
-      <color rgb="FFFF0000"/>
     </mruColors>
   </colors>
   <extLst>
@@ -3445,8 +3474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:X452"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="227" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V8" sqref="V8"/>
+    <sheetView tabSelected="1" zoomScale="227" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D429" sqref="D429"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -4043,25 +4072,25 @@
   <sheetData>
     <row r="2" spans="2:20" ht="16">
       <c r="B2" s="2"/>
-      <c r="C2" s="59" t="s">
+      <c r="C2" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
     </row>
     <row r="3" spans="2:20" ht="23">
       <c r="B3" s="4"/>
-      <c r="C3" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
+      <c r="C3" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="5"/>
@@ -4076,14 +4105,14 @@
     </row>
     <row r="4" spans="2:20" ht="23">
       <c r="B4" s="6"/>
-      <c r="C4" s="59" t="s">
+      <c r="C4" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
-      <c r="H4" s="59"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="58"/>
+      <c r="H4" s="58"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
       <c r="K4" s="5"/>
@@ -4098,14 +4127,14 @@
     </row>
     <row r="5" spans="2:20" ht="23">
       <c r="B5" s="6"/>
-      <c r="C5" s="59" t="s">
+      <c r="C5" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="59"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="58"/>
+      <c r="H5" s="58"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="5"/>
@@ -4120,14 +4149,14 @@
     </row>
     <row r="6" spans="2:20" ht="23">
       <c r="B6" s="6"/>
-      <c r="C6" s="59" t="s">
+      <c r="C6" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="59"/>
-      <c r="H6" s="59"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="58"/>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
       <c r="K6" s="5"/>
@@ -4142,14 +4171,14 @@
     </row>
     <row r="7" spans="2:20" ht="30.75" customHeight="1">
       <c r="B7" s="6"/>
-      <c r="C7" s="60" t="s">
+      <c r="C7" s="59" t="s">
         <v>233</v>
       </c>
-      <c r="D7" s="60"/>
-      <c r="E7" s="60"/>
-      <c r="F7" s="60"/>
-      <c r="G7" s="60"/>
-      <c r="H7" s="60"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="59"/>
+      <c r="G7" s="59"/>
+      <c r="H7" s="59"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
       <c r="K7" s="5"/>
@@ -4164,12 +4193,12 @@
     </row>
     <row r="8" spans="2:20" ht="48" customHeight="1">
       <c r="B8" s="6"/>
-      <c r="C8" s="58" t="s">
+      <c r="C8" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="58"/>
-      <c r="E8" s="58"/>
-      <c r="F8" s="58"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="57"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -4240,7 +4269,7 @@
       <c r="C11" s="17" t="s">
         <v>345</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="60" t="s">
         <v>15</v>
       </c>
       <c r="E11" s="19" t="s">
@@ -4296,7 +4325,7 @@
       <c r="C13" s="20" t="s">
         <v>347</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="60" t="s">
         <v>17</v>
       </c>
       <c r="E13" s="19" t="s">
@@ -4352,7 +4381,7 @@
       <c r="C15" s="17" t="s">
         <v>349</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="D15" s="60" t="s">
         <v>791</v>
       </c>
       <c r="E15" s="19" t="s">
@@ -4408,7 +4437,7 @@
       <c r="C17" s="20" t="s">
         <v>351</v>
       </c>
-      <c r="D17" s="18" t="s">
+      <c r="D17" s="60" t="s">
         <v>792</v>
       </c>
       <c r="E17" s="19" t="s">
@@ -4436,7 +4465,7 @@
       <c r="C18" s="17" t="s">
         <v>352</v>
       </c>
-      <c r="D18" s="18" t="s">
+      <c r="D18" s="60" t="s">
         <v>20</v>
       </c>
       <c r="E18" s="19" t="s">
@@ -4464,7 +4493,7 @@
       <c r="C19" s="17" t="s">
         <v>353</v>
       </c>
-      <c r="D19" s="18" t="s">
+      <c r="D19" s="60" t="s">
         <v>239</v>
       </c>
       <c r="E19" s="19" t="s">
@@ -4492,7 +4521,7 @@
       <c r="C20" s="17" t="s">
         <v>354</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="60" t="s">
         <v>248</v>
       </c>
       <c r="E20" s="19" t="s">
@@ -4520,7 +4549,7 @@
       <c r="C21" s="20" t="s">
         <v>355</v>
       </c>
-      <c r="D21" s="18" t="s">
+      <c r="D21" s="60" t="s">
         <v>21</v>
       </c>
       <c r="E21" s="19" t="s">
@@ -4548,7 +4577,7 @@
       <c r="C22" s="17" t="s">
         <v>356</v>
       </c>
-      <c r="D22" s="18" t="s">
+      <c r="D22" s="60" t="s">
         <v>231</v>
       </c>
       <c r="E22" s="19" t="s">
@@ -4576,7 +4605,7 @@
       <c r="C23" s="17" t="s">
         <v>357</v>
       </c>
-      <c r="D23" s="18" t="s">
+      <c r="D23" s="60" t="s">
         <v>232</v>
       </c>
       <c r="E23" s="19" t="s">
@@ -4604,7 +4633,7 @@
       <c r="C24" s="17" t="s">
         <v>358</v>
       </c>
-      <c r="D24" s="18" t="s">
+      <c r="D24" s="60" t="s">
         <v>794</v>
       </c>
       <c r="E24" s="19" t="s">
@@ -4658,7 +4687,7 @@
       <c r="C26" s="17" t="s">
         <v>360</v>
       </c>
-      <c r="D26" s="18" t="s">
+      <c r="D26" s="60" t="s">
         <v>796</v>
       </c>
       <c r="E26" s="19" t="s">
@@ -4686,7 +4715,7 @@
       <c r="C27" s="17" t="s">
         <v>361</v>
       </c>
-      <c r="D27" s="18" t="s">
+      <c r="D27" s="60" t="s">
         <v>797</v>
       </c>
       <c r="E27" s="19" t="s">
@@ -4796,7 +4825,7 @@
       <c r="C31" s="20" t="s">
         <v>365</v>
       </c>
-      <c r="D31" s="18" t="s">
+      <c r="D31" s="60" t="s">
         <v>250</v>
       </c>
       <c r="E31" s="40" t="s">
@@ -4824,7 +4853,7 @@
       <c r="C32" s="17" t="s">
         <v>366</v>
       </c>
-      <c r="D32" s="18" t="s">
+      <c r="D32" s="60" t="s">
         <v>235</v>
       </c>
       <c r="E32" s="40" t="s">
@@ -4880,7 +4909,7 @@
       <c r="C34" s="17" t="s">
         <v>368</v>
       </c>
-      <c r="D34" s="18" t="s">
+      <c r="D34" s="60" t="s">
         <v>824</v>
       </c>
       <c r="E34" s="40" t="s">
@@ -4908,13 +4937,13 @@
       <c r="C35" s="17" t="s">
         <v>369</v>
       </c>
-      <c r="D35" s="18" t="s">
+      <c r="D35" s="60" t="s">
         <v>238</v>
       </c>
       <c r="E35" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="F35" s="48">
+      <c r="F35" s="47">
         <v>1</v>
       </c>
       <c r="G35" s="41"/>
@@ -4936,13 +4965,13 @@
       <c r="C36" s="20" t="s">
         <v>370</v>
       </c>
-      <c r="D36" s="18" t="s">
+      <c r="D36" s="60" t="s">
         <v>319</v>
       </c>
       <c r="E36" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="F36" s="48">
+      <c r="F36" s="47">
         <v>1</v>
       </c>
       <c r="G36" s="41"/>
@@ -4964,13 +4993,13 @@
       <c r="C37" s="17" t="s">
         <v>371</v>
       </c>
-      <c r="D37" s="18" t="s">
+      <c r="D37" s="60" t="s">
         <v>234</v>
       </c>
-      <c r="E37" s="48" t="s">
+      <c r="E37" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="F37" s="48">
+      <c r="F37" s="47">
         <v>1</v>
       </c>
       <c r="G37" s="41"/>
@@ -4995,10 +5024,10 @@
       <c r="D38" s="18" t="s">
         <v>287</v>
       </c>
-      <c r="E38" s="48" t="s">
+      <c r="E38" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="F38" s="48">
+      <c r="F38" s="47">
         <v>1</v>
       </c>
       <c r="G38" s="41"/>
@@ -5020,13 +5049,13 @@
       <c r="C39" s="20" t="s">
         <v>373</v>
       </c>
-      <c r="D39" s="18" t="s">
+      <c r="D39" s="60" t="s">
         <v>288</v>
       </c>
-      <c r="E39" s="48" t="s">
+      <c r="E39" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="F39" s="48">
+      <c r="F39" s="47">
         <v>1</v>
       </c>
       <c r="G39" s="41"/>
@@ -5048,13 +5077,13 @@
       <c r="C40" s="17" t="s">
         <v>374</v>
       </c>
-      <c r="D40" s="18" t="s">
+      <c r="D40" s="60" t="s">
         <v>290</v>
       </c>
-      <c r="E40" s="48" t="s">
+      <c r="E40" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="F40" s="48">
+      <c r="F40" s="47">
         <v>1</v>
       </c>
       <c r="G40" s="41"/>
@@ -5076,13 +5105,13 @@
       <c r="C41" s="17" t="s">
         <v>375</v>
       </c>
-      <c r="D41" s="18" t="s">
+      <c r="D41" s="60" t="s">
         <v>289</v>
       </c>
-      <c r="E41" s="48" t="s">
+      <c r="E41" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="F41" s="48">
+      <c r="F41" s="47">
         <v>1</v>
       </c>
       <c r="G41" s="41"/>
@@ -5104,13 +5133,13 @@
       <c r="C42" s="20" t="s">
         <v>376</v>
       </c>
-      <c r="D42" s="18" t="s">
+      <c r="D42" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="E42" s="48" t="s">
+      <c r="E42" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="F42" s="48">
+      <c r="F42" s="47">
         <v>1</v>
       </c>
       <c r="G42" s="41"/>
@@ -5132,13 +5161,13 @@
       <c r="C43" s="17" t="s">
         <v>377</v>
       </c>
-      <c r="D43" s="18" t="s">
+      <c r="D43" s="60" t="s">
         <v>321</v>
       </c>
-      <c r="E43" s="48" t="s">
+      <c r="E43" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="F43" s="48">
+      <c r="F43" s="47">
         <v>1</v>
       </c>
       <c r="G43" s="41"/>
@@ -5160,13 +5189,13 @@
       <c r="C44" s="17" t="s">
         <v>378</v>
       </c>
-      <c r="D44" s="18" t="s">
+      <c r="D44" s="60" t="s">
         <v>323</v>
       </c>
-      <c r="E44" s="48" t="s">
+      <c r="E44" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="F44" s="48">
+      <c r="F44" s="47">
         <v>1</v>
       </c>
       <c r="G44" s="41"/>
@@ -5188,13 +5217,13 @@
       <c r="C45" s="20" t="s">
         <v>379</v>
       </c>
-      <c r="D45" s="18" t="s">
+      <c r="D45" s="60" t="s">
         <v>412</v>
       </c>
-      <c r="E45" s="48" t="s">
+      <c r="E45" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="F45" s="48">
+      <c r="F45" s="47">
         <v>1</v>
       </c>
       <c r="G45" s="41"/>
@@ -5216,13 +5245,13 @@
       <c r="C46" s="17" t="s">
         <v>380</v>
       </c>
-      <c r="D46" s="18" t="s">
+      <c r="D46" s="60" t="s">
         <v>333</v>
       </c>
-      <c r="E46" s="48" t="s">
+      <c r="E46" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="F46" s="48">
+      <c r="F46" s="47">
         <v>1</v>
       </c>
       <c r="G46" s="41"/>
@@ -5244,13 +5273,13 @@
       <c r="C47" s="17" t="s">
         <v>381</v>
       </c>
-      <c r="D47" s="18" t="s">
+      <c r="D47" s="60" t="s">
         <v>240</v>
       </c>
-      <c r="E47" s="48" t="s">
+      <c r="E47" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="F47" s="48">
+      <c r="F47" s="47">
         <v>1</v>
       </c>
       <c r="G47" s="41"/>
@@ -5328,7 +5357,7 @@
       <c r="C50" s="17" t="s">
         <v>459</v>
       </c>
-      <c r="D50" s="18" t="s">
+      <c r="D50" s="60" t="s">
         <v>418</v>
       </c>
       <c r="E50" s="19" t="s">
@@ -5440,11 +5469,11 @@
       <c r="C54" s="13">
         <v>2</v>
       </c>
-      <c r="D54" s="54" t="s">
+      <c r="D54" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="E54" s="55"/>
-      <c r="F54" s="55"/>
+      <c r="E54" s="54"/>
+      <c r="F54" s="54"/>
     </row>
     <row r="55" spans="3:20">
       <c r="C55" s="20" t="s">
@@ -5478,7 +5507,7 @@
       <c r="C56" s="20" t="s">
         <v>384</v>
       </c>
-      <c r="D56" s="18" t="s">
+      <c r="D56" s="60" t="s">
         <v>283</v>
       </c>
       <c r="E56" s="19" t="s">
@@ -5506,7 +5535,7 @@
       <c r="C57" s="20" t="s">
         <v>385</v>
       </c>
-      <c r="D57" s="18" t="s">
+      <c r="D57" s="60" t="s">
         <v>284</v>
       </c>
       <c r="E57" s="19" t="s">
@@ -5534,7 +5563,7 @@
       <c r="C58" s="20" t="s">
         <v>463</v>
       </c>
-      <c r="D58" s="18" t="s">
+      <c r="D58" s="60" t="s">
         <v>437</v>
       </c>
       <c r="E58" s="19" t="s">
@@ -5562,7 +5591,7 @@
       <c r="C59" s="20" t="s">
         <v>464</v>
       </c>
-      <c r="D59" s="18" t="s">
+      <c r="D59" s="60" t="s">
         <v>438</v>
       </c>
       <c r="E59" s="19" t="s">
@@ -5590,17 +5619,17 @@
       <c r="C60" s="13">
         <v>3</v>
       </c>
-      <c r="D60" s="54" t="s">
+      <c r="D60" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="E60" s="55"/>
-      <c r="F60" s="55"/>
+      <c r="E60" s="54"/>
+      <c r="F60" s="54"/>
     </row>
     <row r="61" spans="3:20">
       <c r="C61" s="20" t="s">
         <v>386</v>
       </c>
-      <c r="D61" s="18" t="s">
+      <c r="D61" s="60" t="s">
         <v>421</v>
       </c>
       <c r="E61" s="19" t="s">
@@ -5614,7 +5643,7 @@
       <c r="C62" s="20" t="s">
         <v>389</v>
       </c>
-      <c r="D62" s="18" t="s">
+      <c r="D62" s="60" t="s">
         <v>422</v>
       </c>
       <c r="E62" s="19" t="s">
@@ -5628,7 +5657,7 @@
       <c r="C63" s="17" t="s">
         <v>390</v>
       </c>
-      <c r="D63" s="18" t="s">
+      <c r="D63" s="60" t="s">
         <v>27</v>
       </c>
       <c r="E63" s="23" t="s">
@@ -5642,7 +5671,7 @@
       <c r="C64" s="20" t="s">
         <v>391</v>
       </c>
-      <c r="D64" s="18" t="s">
+      <c r="D64" s="60" t="s">
         <v>423</v>
       </c>
       <c r="E64" s="19" t="s">
@@ -5670,7 +5699,7 @@
       <c r="C65" s="17" t="s">
         <v>392</v>
       </c>
-      <c r="D65" s="18" t="s">
+      <c r="D65" s="60" t="s">
         <v>424</v>
       </c>
       <c r="E65" s="19" t="s">
@@ -5684,7 +5713,7 @@
       <c r="C66" s="20" t="s">
         <v>393</v>
       </c>
-      <c r="D66" s="18" t="s">
+      <c r="D66" s="60" t="s">
         <v>307</v>
       </c>
       <c r="E66" s="19" t="s">
@@ -5698,7 +5727,7 @@
       <c r="C67" s="17" t="s">
         <v>394</v>
       </c>
-      <c r="D67" s="18" t="s">
+      <c r="D67" s="60" t="s">
         <v>309</v>
       </c>
       <c r="E67" s="19" t="s">
@@ -5712,7 +5741,7 @@
       <c r="C68" s="20" t="s">
         <v>395</v>
       </c>
-      <c r="D68" s="18" t="s">
+      <c r="D68" s="60" t="s">
         <v>433</v>
       </c>
       <c r="E68" s="19" t="s">
@@ -5726,7 +5755,7 @@
       <c r="C69" s="17" t="s">
         <v>396</v>
       </c>
-      <c r="D69" s="18" t="s">
+      <c r="D69" s="60" t="s">
         <v>435</v>
       </c>
       <c r="E69" s="19" t="s">
@@ -5740,7 +5769,7 @@
       <c r="C70" s="20" t="s">
         <v>397</v>
       </c>
-      <c r="D70" s="18" t="s">
+      <c r="D70" s="60" t="s">
         <v>29</v>
       </c>
       <c r="E70" s="23" t="s">
@@ -5755,7 +5784,7 @@
       <c r="C71" s="17" t="s">
         <v>398</v>
       </c>
-      <c r="D71" s="18" t="s">
+      <c r="D71" s="60" t="s">
         <v>30</v>
       </c>
       <c r="E71" s="19" t="s">
@@ -5769,7 +5798,7 @@
       <c r="C72" s="20" t="s">
         <v>399</v>
       </c>
-      <c r="D72" s="26" t="s">
+      <c r="D72" s="61" t="s">
         <v>244</v>
       </c>
       <c r="E72" s="40" t="s">
@@ -5797,7 +5826,7 @@
       <c r="C73" s="17" t="s">
         <v>400</v>
       </c>
-      <c r="D73" s="18" t="s">
+      <c r="D73" s="60" t="s">
         <v>31</v>
       </c>
       <c r="E73" s="19" t="s">
@@ -5825,7 +5854,7 @@
       <c r="C74" s="20" t="s">
         <v>401</v>
       </c>
-      <c r="D74" s="18" t="s">
+      <c r="D74" s="60" t="s">
         <v>420</v>
       </c>
       <c r="E74" s="19" t="s">
@@ -5853,7 +5882,7 @@
       <c r="C75" s="17" t="s">
         <v>402</v>
       </c>
-      <c r="D75" s="18" t="s">
+      <c r="D75" s="60" t="s">
         <v>245</v>
       </c>
       <c r="E75" s="19" t="s">
@@ -5882,7 +5911,7 @@
       <c r="C76" s="17" t="s">
         <v>403</v>
       </c>
-      <c r="D76" s="18" t="s">
+      <c r="D76" s="60" t="s">
         <v>275</v>
       </c>
       <c r="E76" s="19" t="s">
@@ -5910,7 +5939,7 @@
       <c r="C77" s="20" t="s">
         <v>404</v>
       </c>
-      <c r="D77" s="18" t="s">
+      <c r="D77" s="60" t="s">
         <v>246</v>
       </c>
       <c r="E77" s="19" t="s">
@@ -5938,7 +5967,7 @@
       <c r="C78" s="17" t="s">
         <v>405</v>
       </c>
-      <c r="D78" s="26" t="s">
+      <c r="D78" s="61" t="s">
         <v>32</v>
       </c>
       <c r="E78" s="40" t="s">
@@ -5966,7 +5995,7 @@
       <c r="C79" s="20" t="s">
         <v>406</v>
       </c>
-      <c r="D79" s="26" t="s">
+      <c r="D79" s="61" t="s">
         <v>33</v>
       </c>
       <c r="E79" s="40" t="s">
@@ -5994,7 +6023,7 @@
       <c r="C80" s="17" t="s">
         <v>407</v>
       </c>
-      <c r="D80" s="26" t="s">
+      <c r="D80" s="61" t="s">
         <v>285</v>
       </c>
       <c r="E80" s="40" t="s">
@@ -6022,7 +6051,7 @@
       <c r="C81" s="20" t="s">
         <v>408</v>
       </c>
-      <c r="D81" s="26" t="s">
+      <c r="D81" s="61" t="s">
         <v>417</v>
       </c>
       <c r="E81" s="40" t="s">
@@ -6050,7 +6079,7 @@
       <c r="C82" s="17" t="s">
         <v>409</v>
       </c>
-      <c r="D82" s="26" t="s">
+      <c r="D82" s="61" t="s">
         <v>324</v>
       </c>
       <c r="E82" s="40" t="s">
@@ -6078,7 +6107,7 @@
       <c r="C83" s="20" t="s">
         <v>410</v>
       </c>
-      <c r="D83" s="26" t="s">
+      <c r="D83" s="61" t="s">
         <v>326</v>
       </c>
       <c r="E83" s="40" t="s">
@@ -6092,7 +6121,7 @@
       <c r="C84" s="17" t="s">
         <v>411</v>
       </c>
-      <c r="D84" s="26" t="s">
+      <c r="D84" s="61" t="s">
         <v>337</v>
       </c>
       <c r="E84" s="40" t="s">
@@ -6120,7 +6149,7 @@
       <c r="C85" s="20" t="s">
         <v>465</v>
       </c>
-      <c r="D85" s="26" t="s">
+      <c r="D85" s="61" t="s">
         <v>457</v>
       </c>
       <c r="E85" s="40" t="s">
@@ -6134,7 +6163,7 @@
       <c r="C86" s="17" t="s">
         <v>466</v>
       </c>
-      <c r="D86" s="26" t="s">
+      <c r="D86" s="61" t="s">
         <v>34</v>
       </c>
       <c r="E86" s="40" t="s">
@@ -6204,7 +6233,7 @@
       <c r="C89" s="17" t="s">
         <v>469</v>
       </c>
-      <c r="D89" s="26" t="s">
+      <c r="D89" s="61" t="s">
         <v>416</v>
       </c>
       <c r="E89" s="40" t="s">
@@ -6218,7 +6247,7 @@
       <c r="C90" s="20" t="s">
         <v>470</v>
       </c>
-      <c r="D90" s="26" t="s">
+      <c r="D90" s="61" t="s">
         <v>434</v>
       </c>
       <c r="E90" s="40" t="s">
@@ -6232,7 +6261,7 @@
       <c r="C91" s="17" t="s">
         <v>471</v>
       </c>
-      <c r="D91" s="26" t="s">
+      <c r="D91" s="61" t="s">
         <v>827</v>
       </c>
       <c r="E91" s="40" t="s">
@@ -6298,7 +6327,7 @@
       <c r="C95" s="20" t="s">
         <v>473</v>
       </c>
-      <c r="D95" s="18" t="s">
+      <c r="D95" s="60" t="s">
         <v>38</v>
       </c>
       <c r="E95" s="19" t="s">
@@ -6326,7 +6355,7 @@
       <c r="C96" s="20" t="s">
         <v>474</v>
       </c>
-      <c r="D96" s="18" t="s">
+      <c r="D96" s="60" t="s">
         <v>39</v>
       </c>
       <c r="E96" s="19" t="s">
@@ -6354,7 +6383,7 @@
       <c r="C97" s="20" t="s">
         <v>475</v>
       </c>
-      <c r="D97" s="18" t="s">
+      <c r="D97" s="60" t="s">
         <v>40</v>
       </c>
       <c r="E97" s="19" t="s">
@@ -6382,7 +6411,7 @@
       <c r="C98" s="20" t="s">
         <v>476</v>
       </c>
-      <c r="D98" s="27" t="s">
+      <c r="D98" s="62" t="s">
         <v>41</v>
       </c>
       <c r="E98" s="19" t="s">
@@ -6438,7 +6467,7 @@
       <c r="C100" s="20" t="s">
         <v>478</v>
       </c>
-      <c r="D100" s="18" t="s">
+      <c r="D100" s="60" t="s">
         <v>304</v>
       </c>
       <c r="E100" s="19" t="s">
@@ -6466,7 +6495,7 @@
       <c r="C101" s="20" t="s">
         <v>479</v>
       </c>
-      <c r="D101" s="18" t="s">
+      <c r="D101" s="60" t="s">
         <v>303</v>
       </c>
       <c r="E101" s="19" t="s">
@@ -6522,7 +6551,7 @@
       <c r="C103" s="20" t="s">
         <v>481</v>
       </c>
-      <c r="D103" s="18" t="s">
+      <c r="D103" s="60" t="s">
         <v>42</v>
       </c>
       <c r="E103" s="23" t="s">
@@ -6550,7 +6579,7 @@
       <c r="C104" s="20" t="s">
         <v>482</v>
       </c>
-      <c r="D104" s="18" t="s">
+      <c r="D104" s="60" t="s">
         <v>425</v>
       </c>
       <c r="E104" s="23" t="s">
@@ -6578,7 +6607,7 @@
       <c r="C105" s="20" t="s">
         <v>483</v>
       </c>
-      <c r="D105" s="18" t="s">
+      <c r="D105" s="60" t="s">
         <v>306</v>
       </c>
       <c r="E105" s="23" t="s">
@@ -6606,7 +6635,7 @@
       <c r="C106" s="20" t="s">
         <v>484</v>
       </c>
-      <c r="D106" s="18" t="s">
+      <c r="D106" s="60" t="s">
         <v>322</v>
       </c>
       <c r="E106" s="23" t="s">
@@ -6634,7 +6663,7 @@
       <c r="C107" s="20" t="s">
         <v>485</v>
       </c>
-      <c r="D107" s="18" t="s">
+      <c r="D107" s="60" t="s">
         <v>335</v>
       </c>
       <c r="E107" s="23" t="s">
@@ -6662,7 +6691,7 @@
       <c r="C108" s="20" t="s">
         <v>486</v>
       </c>
-      <c r="D108" s="18" t="s">
+      <c r="D108" s="60" t="s">
         <v>338</v>
       </c>
       <c r="E108" s="23" t="s">
@@ -6690,7 +6719,7 @@
       <c r="C109" s="20" t="s">
         <v>487</v>
       </c>
-      <c r="D109" s="18" t="s">
+      <c r="D109" s="60" t="s">
         <v>426</v>
       </c>
       <c r="E109" s="23" t="s">
@@ -6756,7 +6785,7 @@
       <c r="C112" s="20" t="s">
         <v>489</v>
       </c>
-      <c r="D112" s="18" t="s">
+      <c r="D112" s="60" t="s">
         <v>45</v>
       </c>
       <c r="E112" s="19" t="s">
@@ -6784,7 +6813,7 @@
       <c r="C113" s="20" t="s">
         <v>490</v>
       </c>
-      <c r="D113" s="18" t="s">
+      <c r="D113" s="60" t="s">
         <v>46</v>
       </c>
       <c r="E113" s="19" t="s">
@@ -6815,7 +6844,7 @@
       <c r="D114" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="E114" s="49" t="s">
+      <c r="E114" s="48" t="s">
         <v>8</v>
       </c>
       <c r="F114" s="19">
@@ -6952,7 +6981,7 @@
       <c r="C119" s="20" t="s">
         <v>496</v>
       </c>
-      <c r="D119" s="18" t="s">
+      <c r="D119" s="60" t="s">
         <v>52</v>
       </c>
       <c r="E119" s="19" t="s">
@@ -6980,7 +7009,7 @@
       <c r="C120" s="20" t="s">
         <v>497</v>
       </c>
-      <c r="D120" s="18" t="s">
+      <c r="D120" s="60" t="s">
         <v>53</v>
       </c>
       <c r="E120" s="19" t="s">
@@ -7008,7 +7037,7 @@
       <c r="C121" s="20" t="s">
         <v>498</v>
       </c>
-      <c r="D121" s="18" t="s">
+      <c r="D121" s="60" t="s">
         <v>54</v>
       </c>
       <c r="E121" s="19" t="s">
@@ -7036,7 +7065,7 @@
       <c r="C122" s="20" t="s">
         <v>499</v>
       </c>
-      <c r="D122" s="18" t="s">
+      <c r="D122" s="60" t="s">
         <v>55</v>
       </c>
       <c r="E122" s="19" t="s">
@@ -7064,7 +7093,7 @@
       <c r="C123" s="20" t="s">
         <v>500</v>
       </c>
-      <c r="D123" s="18" t="s">
+      <c r="D123" s="60" t="s">
         <v>56</v>
       </c>
       <c r="E123" s="19" t="s">
@@ -7092,7 +7121,7 @@
       <c r="C124" s="20" t="s">
         <v>501</v>
       </c>
-      <c r="D124" s="18" t="s">
+      <c r="D124" s="60" t="s">
         <v>57</v>
       </c>
       <c r="E124" s="19" t="s">
@@ -7120,7 +7149,7 @@
       <c r="C125" s="20" t="s">
         <v>502</v>
       </c>
-      <c r="D125" s="18" t="s">
+      <c r="D125" s="60" t="s">
         <v>58</v>
       </c>
       <c r="E125" s="19" t="s">
@@ -7148,7 +7177,7 @@
       <c r="C126" s="20" t="s">
         <v>503</v>
       </c>
-      <c r="D126" s="18" t="s">
+      <c r="D126" s="60" t="s">
         <v>317</v>
       </c>
       <c r="E126" s="19" t="s">
@@ -7176,7 +7205,7 @@
       <c r="C127" s="20" t="s">
         <v>504</v>
       </c>
-      <c r="D127" s="18" t="s">
+      <c r="D127" s="60" t="s">
         <v>59</v>
       </c>
       <c r="E127" s="19" t="s">
@@ -7204,7 +7233,7 @@
       <c r="C128" s="20" t="s">
         <v>505</v>
       </c>
-      <c r="D128" s="18" t="s">
+      <c r="D128" s="60" t="s">
         <v>60</v>
       </c>
       <c r="E128" s="19" t="s">
@@ -7232,7 +7261,7 @@
       <c r="C129" s="20" t="s">
         <v>506</v>
       </c>
-      <c r="D129" s="18" t="s">
+      <c r="D129" s="60" t="s">
         <v>803</v>
       </c>
       <c r="E129" s="19" t="s">
@@ -7260,7 +7289,7 @@
       <c r="C130" s="20" t="s">
         <v>507</v>
       </c>
-      <c r="D130" s="18" t="s">
+      <c r="D130" s="60" t="s">
         <v>268</v>
       </c>
       <c r="E130" s="19" t="s">
@@ -7288,7 +7317,7 @@
       <c r="C131" s="20" t="s">
         <v>508</v>
       </c>
-      <c r="D131" s="18" t="s">
+      <c r="D131" s="60" t="s">
         <v>251</v>
       </c>
       <c r="E131" s="19" t="s">
@@ -7316,7 +7345,7 @@
       <c r="C132" s="20" t="s">
         <v>509</v>
       </c>
-      <c r="D132" s="18" t="s">
+      <c r="D132" s="60" t="s">
         <v>252</v>
       </c>
       <c r="E132" s="19" t="s">
@@ -7344,7 +7373,7 @@
       <c r="C133" s="20" t="s">
         <v>510</v>
       </c>
-      <c r="D133" s="18" t="s">
+      <c r="D133" s="60" t="s">
         <v>799</v>
       </c>
       <c r="E133" s="19" t="s">
@@ -7372,7 +7401,7 @@
       <c r="C134" s="20" t="s">
         <v>511</v>
       </c>
-      <c r="D134" s="18" t="s">
+      <c r="D134" s="60" t="s">
         <v>800</v>
       </c>
       <c r="E134" s="19" t="s">
@@ -7400,7 +7429,7 @@
       <c r="C135" s="20" t="s">
         <v>512</v>
       </c>
-      <c r="D135" s="18" t="s">
+      <c r="D135" s="60" t="s">
         <v>254</v>
       </c>
       <c r="E135" s="19" t="s">
@@ -7428,7 +7457,7 @@
       <c r="C136" s="20" t="s">
         <v>513</v>
       </c>
-      <c r="D136" s="18" t="s">
+      <c r="D136" s="60" t="s">
         <v>253</v>
       </c>
       <c r="E136" s="19" t="s">
@@ -7456,7 +7485,7 @@
       <c r="C137" s="20" t="s">
         <v>514</v>
       </c>
-      <c r="D137" s="18" t="s">
+      <c r="D137" s="60" t="s">
         <v>312</v>
       </c>
       <c r="E137" s="19" t="s">
@@ -7484,7 +7513,7 @@
       <c r="C138" s="20" t="s">
         <v>515</v>
       </c>
-      <c r="D138" s="18" t="s">
+      <c r="D138" s="60" t="s">
         <v>256</v>
       </c>
       <c r="E138" s="19" t="s">
@@ -7512,7 +7541,7 @@
       <c r="C139" s="20" t="s">
         <v>516</v>
       </c>
-      <c r="D139" s="18" t="s">
+      <c r="D139" s="60" t="s">
         <v>804</v>
       </c>
       <c r="E139" s="19" t="s">
@@ -7540,7 +7569,7 @@
       <c r="C140" s="20" t="s">
         <v>517</v>
       </c>
-      <c r="D140" s="18" t="s">
+      <c r="D140" s="60" t="s">
         <v>805</v>
       </c>
       <c r="E140" s="19" t="s">
@@ -7568,7 +7597,7 @@
       <c r="C141" s="20" t="s">
         <v>518</v>
       </c>
-      <c r="D141" s="18" t="s">
+      <c r="D141" s="60" t="s">
         <v>806</v>
       </c>
       <c r="E141" s="19" t="s">
@@ -7596,7 +7625,7 @@
       <c r="C142" s="20" t="s">
         <v>519</v>
       </c>
-      <c r="D142" s="18" t="s">
+      <c r="D142" s="60" t="s">
         <v>61</v>
       </c>
       <c r="E142" s="19" t="s">
@@ -7624,7 +7653,7 @@
       <c r="C143" s="20" t="s">
         <v>520</v>
       </c>
-      <c r="D143" s="18" t="s">
+      <c r="D143" s="60" t="s">
         <v>62</v>
       </c>
       <c r="E143" s="19" t="s">
@@ -7736,7 +7765,7 @@
       <c r="C147" s="20" t="s">
         <v>524</v>
       </c>
-      <c r="D147" s="18" t="s">
+      <c r="D147" s="60" t="s">
         <v>802</v>
       </c>
       <c r="E147" s="19" t="s">
@@ -7764,7 +7793,7 @@
       <c r="C148" s="20" t="s">
         <v>525</v>
       </c>
-      <c r="D148" s="18" t="s">
+      <c r="D148" s="60" t="s">
         <v>310</v>
       </c>
       <c r="E148" s="19" t="s">
@@ -7792,7 +7821,7 @@
       <c r="C149" s="20" t="s">
         <v>526</v>
       </c>
-      <c r="D149" s="18" t="s">
+      <c r="D149" s="60" t="s">
         <v>439</v>
       </c>
       <c r="E149" s="19" t="s">
@@ -7820,7 +7849,7 @@
       <c r="C150" s="20" t="s">
         <v>801</v>
       </c>
-      <c r="D150" s="18" t="s">
+      <c r="D150" s="63" t="s">
         <v>318</v>
       </c>
       <c r="E150" s="19" t="s">
@@ -7858,10 +7887,10 @@
       <c r="C152" s="20" t="s">
         <v>387</v>
       </c>
-      <c r="D152" s="18" t="s">
+      <c r="D152" s="60" t="s">
         <v>66</v>
       </c>
-      <c r="E152" s="50" t="s">
+      <c r="E152" s="49" t="s">
         <v>8</v>
       </c>
       <c r="F152" s="19">
@@ -7872,10 +7901,10 @@
       <c r="C153" s="20" t="s">
         <v>527</v>
       </c>
-      <c r="D153" s="18" t="s">
+      <c r="D153" s="60" t="s">
         <v>67</v>
       </c>
-      <c r="E153" s="50" t="s">
+      <c r="E153" s="49" t="s">
         <v>8</v>
       </c>
       <c r="F153" s="19">
@@ -7900,10 +7929,10 @@
       <c r="C154" s="20" t="s">
         <v>528</v>
       </c>
-      <c r="D154" s="18" t="s">
+      <c r="D154" s="60" t="s">
         <v>68</v>
       </c>
-      <c r="E154" s="50" t="s">
+      <c r="E154" s="49" t="s">
         <v>8</v>
       </c>
       <c r="F154" s="19">
@@ -7928,10 +7957,10 @@
       <c r="C155" s="20" t="s">
         <v>529</v>
       </c>
-      <c r="D155" s="18" t="s">
+      <c r="D155" s="60" t="s">
         <v>69</v>
       </c>
-      <c r="E155" s="50" t="s">
+      <c r="E155" s="49" t="s">
         <v>8</v>
       </c>
       <c r="F155" s="19">
@@ -7942,10 +7971,10 @@
       <c r="C156" s="20" t="s">
         <v>530</v>
       </c>
-      <c r="D156" s="18" t="s">
+      <c r="D156" s="60" t="s">
         <v>70</v>
       </c>
-      <c r="E156" s="50" t="s">
+      <c r="E156" s="49" t="s">
         <v>8</v>
       </c>
       <c r="F156" s="19">
@@ -7956,10 +7985,10 @@
       <c r="C157" s="20" t="s">
         <v>531</v>
       </c>
-      <c r="D157" s="18" t="s">
+      <c r="D157" s="60" t="s">
         <v>71</v>
       </c>
-      <c r="E157" s="50" t="s">
+      <c r="E157" s="49" t="s">
         <v>8</v>
       </c>
       <c r="F157" s="19">
@@ -7970,10 +7999,10 @@
       <c r="C158" s="20" t="s">
         <v>532</v>
       </c>
-      <c r="D158" s="18" t="s">
+      <c r="D158" s="60" t="s">
         <v>72</v>
       </c>
-      <c r="E158" s="50" t="s">
+      <c r="E158" s="49" t="s">
         <v>8</v>
       </c>
       <c r="F158" s="19">
@@ -7984,10 +8013,10 @@
       <c r="C159" s="20" t="s">
         <v>533</v>
       </c>
-      <c r="D159" s="18" t="s">
+      <c r="D159" s="60" t="s">
         <v>73</v>
       </c>
-      <c r="E159" s="50" t="s">
+      <c r="E159" s="49" t="s">
         <v>8</v>
       </c>
       <c r="F159" s="19">
@@ -7998,10 +8027,10 @@
       <c r="C160" s="20" t="s">
         <v>534</v>
       </c>
-      <c r="D160" s="18" t="s">
+      <c r="D160" s="60" t="s">
         <v>74</v>
       </c>
-      <c r="E160" s="50" t="s">
+      <c r="E160" s="49" t="s">
         <v>8</v>
       </c>
       <c r="F160" s="19">
@@ -8012,10 +8041,10 @@
       <c r="C161" s="20" t="s">
         <v>535</v>
       </c>
-      <c r="D161" s="18" t="s">
+      <c r="D161" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="E161" s="50" t="s">
+      <c r="E161" s="49" t="s">
         <v>8</v>
       </c>
       <c r="F161" s="19">
@@ -8026,10 +8055,10 @@
       <c r="C162" s="20" t="s">
         <v>536</v>
       </c>
-      <c r="D162" s="18" t="s">
+      <c r="D162" s="60" t="s">
         <v>814</v>
       </c>
-      <c r="E162" s="50" t="s">
+      <c r="E162" s="49" t="s">
         <v>8</v>
       </c>
       <c r="F162" s="19">
@@ -8040,10 +8069,10 @@
       <c r="C163" s="20" t="s">
         <v>537</v>
       </c>
-      <c r="D163" s="18" t="s">
+      <c r="D163" s="60" t="s">
         <v>76</v>
       </c>
-      <c r="E163" s="50" t="s">
+      <c r="E163" s="49" t="s">
         <v>8</v>
       </c>
       <c r="F163" s="19">
@@ -8054,10 +8083,10 @@
       <c r="C164" s="20" t="s">
         <v>538</v>
       </c>
-      <c r="D164" s="18" t="s">
+      <c r="D164" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="E164" s="50" t="s">
+      <c r="E164" s="49" t="s">
         <v>28</v>
       </c>
       <c r="F164" s="19">
@@ -8068,10 +8097,10 @@
       <c r="C165" s="20" t="s">
         <v>539</v>
       </c>
-      <c r="D165" s="18" t="s">
+      <c r="D165" s="60" t="s">
         <v>78</v>
       </c>
-      <c r="E165" s="50" t="s">
+      <c r="E165" s="49" t="s">
         <v>8</v>
       </c>
       <c r="F165" s="19">
@@ -8082,10 +8111,10 @@
       <c r="C166" s="20" t="s">
         <v>540</v>
       </c>
-      <c r="D166" s="18" t="s">
+      <c r="D166" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="E166" s="50" t="s">
+      <c r="E166" s="49" t="s">
         <v>8</v>
       </c>
       <c r="F166" s="19">
@@ -8096,10 +8125,10 @@
       <c r="C167" s="20" t="s">
         <v>541</v>
       </c>
-      <c r="D167" s="18" t="s">
+      <c r="D167" s="60" t="s">
         <v>80</v>
       </c>
-      <c r="E167" s="50" t="s">
+      <c r="E167" s="49" t="s">
         <v>8</v>
       </c>
       <c r="F167" s="19">
@@ -8110,10 +8139,10 @@
       <c r="C168" s="20" t="s">
         <v>542</v>
       </c>
-      <c r="D168" s="18" t="s">
+      <c r="D168" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="E168" s="50" t="s">
+      <c r="E168" s="49" t="s">
         <v>8</v>
       </c>
       <c r="F168" s="19">
@@ -8124,10 +8153,10 @@
       <c r="C169" s="20" t="s">
         <v>543</v>
       </c>
-      <c r="D169" s="18" t="s">
+      <c r="D169" s="60" t="s">
         <v>82</v>
       </c>
-      <c r="E169" s="50" t="s">
+      <c r="E169" s="49" t="s">
         <v>8</v>
       </c>
       <c r="F169" s="19">
@@ -8138,10 +8167,10 @@
       <c r="C170" s="20" t="s">
         <v>544</v>
       </c>
-      <c r="D170" s="18" t="s">
+      <c r="D170" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="E170" s="50" t="s">
+      <c r="E170" s="49" t="s">
         <v>28</v>
       </c>
       <c r="F170" s="19">
@@ -8154,10 +8183,10 @@
       <c r="C171" s="20" t="s">
         <v>545</v>
       </c>
-      <c r="D171" s="18" t="s">
+      <c r="D171" s="60" t="s">
         <v>84</v>
       </c>
-      <c r="E171" s="50" t="s">
+      <c r="E171" s="49" t="s">
         <v>8</v>
       </c>
       <c r="F171" s="19">
@@ -8184,10 +8213,10 @@
       <c r="C172" s="20" t="s">
         <v>546</v>
       </c>
-      <c r="D172" s="18" t="s">
+      <c r="D172" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="E172" s="50" t="s">
+      <c r="E172" s="49" t="s">
         <v>8</v>
       </c>
       <c r="F172" s="19">
@@ -8212,10 +8241,10 @@
       <c r="C173" s="20" t="s">
         <v>547</v>
       </c>
-      <c r="D173" s="18" t="s">
+      <c r="D173" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="E173" s="50" t="s">
+      <c r="E173" s="49" t="s">
         <v>8</v>
       </c>
       <c r="F173" s="19">
@@ -8226,10 +8255,10 @@
       <c r="C174" s="20" t="s">
         <v>548</v>
       </c>
-      <c r="D174" s="18" t="s">
+      <c r="D174" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="E174" s="50" t="s">
+      <c r="E174" s="49" t="s">
         <v>8</v>
       </c>
       <c r="F174" s="19">
@@ -8240,10 +8269,10 @@
       <c r="C175" s="20" t="s">
         <v>549</v>
       </c>
-      <c r="D175" s="18" t="s">
+      <c r="D175" s="60" t="s">
         <v>88</v>
       </c>
-      <c r="E175" s="50" t="s">
+      <c r="E175" s="49" t="s">
         <v>8</v>
       </c>
       <c r="F175" s="19">
@@ -8390,7 +8419,7 @@
       <c r="C185" s="20" t="s">
         <v>558</v>
       </c>
-      <c r="D185" s="34" t="s">
+      <c r="D185" s="64" t="s">
         <v>96</v>
       </c>
       <c r="E185" s="28" t="s">
@@ -8404,7 +8433,7 @@
       <c r="C186" s="20" t="s">
         <v>559</v>
       </c>
-      <c r="D186" s="34" t="s">
+      <c r="D186" s="64" t="s">
         <v>97</v>
       </c>
       <c r="E186" s="28" t="s">
@@ -8418,7 +8447,7 @@
       <c r="C187" s="20" t="s">
         <v>560</v>
       </c>
-      <c r="D187" s="34" t="s">
+      <c r="D187" s="64" t="s">
         <v>98</v>
       </c>
       <c r="E187" s="28" t="s">
@@ -9380,7 +9409,7 @@
       <c r="C252" s="20" t="s">
         <v>624</v>
       </c>
-      <c r="D252" s="18" t="s">
+      <c r="D252" s="60" t="s">
         <v>261</v>
       </c>
       <c r="E252" s="19" t="s">
@@ -9408,7 +9437,7 @@
       <c r="C253" s="20" t="s">
         <v>625</v>
       </c>
-      <c r="D253" s="18" t="s">
+      <c r="D253" s="60" t="s">
         <v>427</v>
       </c>
       <c r="E253" s="19" t="s">
@@ -9436,7 +9465,7 @@
       <c r="C254" s="20" t="s">
         <v>626</v>
       </c>
-      <c r="D254" s="18" t="s">
+      <c r="D254" s="60" t="s">
         <v>262</v>
       </c>
       <c r="E254" s="19" t="s">
@@ -9464,7 +9493,7 @@
       <c r="C255" s="20" t="s">
         <v>627</v>
       </c>
-      <c r="D255" s="18" t="s">
+      <c r="D255" s="60" t="s">
         <v>147</v>
       </c>
       <c r="E255" s="19" t="s">
@@ -9492,7 +9521,7 @@
       <c r="C256" s="20" t="s">
         <v>628</v>
       </c>
-      <c r="D256" s="18" t="s">
+      <c r="D256" s="60" t="s">
         <v>148</v>
       </c>
       <c r="E256" s="19" t="s">
@@ -9520,7 +9549,7 @@
       <c r="C257" s="20" t="s">
         <v>629</v>
       </c>
-      <c r="D257" s="18" t="s">
+      <c r="D257" s="60" t="s">
         <v>263</v>
       </c>
       <c r="E257" s="19" t="s">
@@ -9558,7 +9587,7 @@
       <c r="C259" s="20" t="s">
         <v>630</v>
       </c>
-      <c r="D259" s="18" t="s">
+      <c r="D259" s="60" t="s">
         <v>150</v>
       </c>
       <c r="E259" s="19" t="s">
@@ -9572,7 +9601,7 @@
       <c r="C260" s="20" t="s">
         <v>631</v>
       </c>
-      <c r="D260" s="18" t="s">
+      <c r="D260" s="60" t="s">
         <v>151</v>
       </c>
       <c r="E260" s="40" t="s">
@@ -9586,7 +9615,7 @@
       <c r="C261" s="20" t="s">
         <v>632</v>
       </c>
-      <c r="D261" s="18" t="s">
+      <c r="D261" s="60" t="s">
         <v>152</v>
       </c>
       <c r="E261" s="19" t="s">
@@ -9614,7 +9643,7 @@
       <c r="C263" s="20" t="s">
         <v>634</v>
       </c>
-      <c r="D263" s="18" t="s">
+      <c r="D263" s="60" t="s">
         <v>154</v>
       </c>
       <c r="E263" s="19" t="s">
@@ -9656,7 +9685,7 @@
       <c r="C266" s="20" t="s">
         <v>637</v>
       </c>
-      <c r="D266" s="18" t="s">
+      <c r="D266" s="60" t="s">
         <v>314</v>
       </c>
       <c r="E266" s="19" t="s">
@@ -9670,7 +9699,7 @@
       <c r="C267" s="20" t="s">
         <v>638</v>
       </c>
-      <c r="D267" s="27" t="s">
+      <c r="D267" s="62" t="s">
         <v>807</v>
       </c>
       <c r="E267" s="19" t="s">
@@ -9698,7 +9727,7 @@
       <c r="C269" s="20" t="s">
         <v>640</v>
       </c>
-      <c r="D269" s="27" t="s">
+      <c r="D269" s="62" t="s">
         <v>431</v>
       </c>
       <c r="E269" s="19" t="s">
@@ -9712,7 +9741,7 @@
       <c r="C270" s="20" t="s">
         <v>641</v>
       </c>
-      <c r="D270" s="27" t="s">
+      <c r="D270" s="62" t="s">
         <v>155</v>
       </c>
       <c r="E270" s="19" t="s">
@@ -9740,7 +9769,7 @@
       <c r="C271" s="20" t="s">
         <v>642</v>
       </c>
-      <c r="D271" s="27" t="s">
+      <c r="D271" s="62" t="s">
         <v>156</v>
       </c>
       <c r="E271" s="19" t="s">
@@ -9768,7 +9797,7 @@
       <c r="C272" s="20" t="s">
         <v>643</v>
       </c>
-      <c r="D272" s="27" t="s">
+      <c r="D272" s="62" t="s">
         <v>315</v>
       </c>
       <c r="E272" s="19" t="s">
@@ -9796,7 +9825,7 @@
       <c r="C273" s="20" t="s">
         <v>644</v>
       </c>
-      <c r="D273" s="27" t="s">
+      <c r="D273" s="62" t="s">
         <v>344</v>
       </c>
       <c r="E273" s="19" t="s">
@@ -9824,7 +9853,7 @@
       <c r="C274" s="20" t="s">
         <v>645</v>
       </c>
-      <c r="D274" s="18" t="s">
+      <c r="D274" s="60" t="s">
         <v>825</v>
       </c>
       <c r="E274" s="19" t="s">
@@ -9852,7 +9881,7 @@
       <c r="C275" s="20" t="s">
         <v>646</v>
       </c>
-      <c r="D275" s="27" t="s">
+      <c r="D275" s="62" t="s">
         <v>157</v>
       </c>
       <c r="E275" s="19" t="s">
@@ -9880,7 +9909,7 @@
       <c r="C276" s="20" t="s">
         <v>647</v>
       </c>
-      <c r="D276" s="18" t="s">
+      <c r="D276" s="60" t="s">
         <v>158</v>
       </c>
       <c r="E276" s="19" t="s">
@@ -9908,7 +9937,7 @@
       <c r="C277" s="20" t="s">
         <v>648</v>
       </c>
-      <c r="D277" s="27" t="s">
+      <c r="D277" s="62" t="s">
         <v>159</v>
       </c>
       <c r="E277" s="19" t="s">
@@ -9936,7 +9965,7 @@
       <c r="C278" s="20" t="s">
         <v>649</v>
       </c>
-      <c r="D278" s="27" t="s">
+      <c r="D278" s="62" t="s">
         <v>838</v>
       </c>
       <c r="E278" s="19" t="s">
@@ -9964,7 +9993,7 @@
       <c r="C279" s="20" t="s">
         <v>650</v>
       </c>
-      <c r="D279" s="27" t="s">
+      <c r="D279" s="62" t="s">
         <v>271</v>
       </c>
       <c r="E279" s="19" t="s">
@@ -9992,7 +10021,7 @@
       <c r="C280" s="20" t="s">
         <v>651</v>
       </c>
-      <c r="D280" s="27" t="s">
+      <c r="D280" s="62" t="s">
         <v>160</v>
       </c>
       <c r="E280" s="19" t="s">
@@ -10048,7 +10077,7 @@
       <c r="C282" s="20" t="s">
         <v>653</v>
       </c>
-      <c r="D282" s="27" t="s">
+      <c r="D282" s="62" t="s">
         <v>162</v>
       </c>
       <c r="E282" s="19" t="s">
@@ -10076,7 +10105,7 @@
       <c r="C283" s="20" t="s">
         <v>654</v>
       </c>
-      <c r="D283" s="18" t="s">
+      <c r="D283" s="60" t="s">
         <v>163</v>
       </c>
       <c r="E283" s="40" t="s">
@@ -10104,7 +10133,7 @@
       <c r="C284" s="20" t="s">
         <v>655</v>
       </c>
-      <c r="D284" s="27" t="s">
+      <c r="D284" s="62" t="s">
         <v>164</v>
       </c>
       <c r="E284" s="19" t="s">
@@ -10132,7 +10161,7 @@
       <c r="C285" s="20" t="s">
         <v>656</v>
       </c>
-      <c r="D285" s="27" t="s">
+      <c r="D285" s="62" t="s">
         <v>165</v>
       </c>
       <c r="E285" s="19" t="s">
@@ -10160,7 +10189,7 @@
       <c r="C286" s="20" t="s">
         <v>657</v>
       </c>
-      <c r="D286" s="27" t="s">
+      <c r="D286" s="62" t="s">
         <v>166</v>
       </c>
       <c r="E286" s="19" t="s">
@@ -10188,7 +10217,7 @@
       <c r="C287" s="20" t="s">
         <v>658</v>
       </c>
-      <c r="D287" s="27" t="s">
+      <c r="D287" s="62" t="s">
         <v>167</v>
       </c>
       <c r="E287" s="19" t="s">
@@ -10216,7 +10245,7 @@
       <c r="C288" s="20" t="s">
         <v>659</v>
       </c>
-      <c r="D288" s="27" t="s">
+      <c r="D288" s="62" t="s">
         <v>430</v>
       </c>
       <c r="E288" s="19" t="s">
@@ -10272,7 +10301,7 @@
       <c r="C290" s="20" t="s">
         <v>661</v>
       </c>
-      <c r="D290" s="27" t="s">
+      <c r="D290" s="62" t="s">
         <v>839</v>
       </c>
       <c r="E290" s="19" t="s">
@@ -10310,7 +10339,7 @@
       <c r="C292" s="20" t="s">
         <v>662</v>
       </c>
-      <c r="D292" s="18" t="s">
+      <c r="D292" s="60" t="s">
         <v>808</v>
       </c>
       <c r="E292" s="19" t="s">
@@ -10338,7 +10367,7 @@
       <c r="C293" s="20" t="s">
         <v>663</v>
       </c>
-      <c r="D293" s="18" t="s">
+      <c r="D293" s="60" t="s">
         <v>341</v>
       </c>
       <c r="E293" s="19" t="s">
@@ -10366,7 +10395,7 @@
       <c r="C294" s="20" t="s">
         <v>664</v>
       </c>
-      <c r="D294" s="18" t="s">
+      <c r="D294" s="60" t="s">
         <v>169</v>
       </c>
       <c r="E294" s="19" t="s">
@@ -10394,7 +10423,7 @@
       <c r="C295" s="20" t="s">
         <v>665</v>
       </c>
-      <c r="D295" s="18" t="s">
+      <c r="D295" s="60" t="s">
         <v>815</v>
       </c>
       <c r="E295" s="40" t="s">
@@ -10422,7 +10451,7 @@
       <c r="C296" s="20" t="s">
         <v>666</v>
       </c>
-      <c r="D296" s="18" t="s">
+      <c r="D296" s="60" t="s">
         <v>816</v>
       </c>
       <c r="E296" s="19" t="s">
@@ -10450,7 +10479,7 @@
       <c r="C297" s="20" t="s">
         <v>667</v>
       </c>
-      <c r="D297" s="18" t="s">
+      <c r="D297" s="60" t="s">
         <v>817</v>
       </c>
       <c r="E297" s="19" t="s">
@@ -10478,7 +10507,7 @@
       <c r="C298" s="20" t="s">
         <v>668</v>
       </c>
-      <c r="D298" s="18" t="s">
+      <c r="D298" s="60" t="s">
         <v>247</v>
       </c>
       <c r="E298" s="19" t="s">
@@ -10534,7 +10563,7 @@
       <c r="C300" s="20" t="s">
         <v>670</v>
       </c>
-      <c r="D300" s="18" t="s">
+      <c r="D300" s="60" t="s">
         <v>818</v>
       </c>
       <c r="E300" s="19" t="s">
@@ -10562,7 +10591,7 @@
       <c r="C301" s="20" t="s">
         <v>671</v>
       </c>
-      <c r="D301" s="18" t="s">
+      <c r="D301" s="60" t="s">
         <v>819</v>
       </c>
       <c r="E301" s="19" t="s">
@@ -10590,7 +10619,7 @@
       <c r="C302" s="20" t="s">
         <v>672</v>
       </c>
-      <c r="D302" s="18" t="s">
+      <c r="D302" s="60" t="s">
         <v>822</v>
       </c>
       <c r="E302" s="19" t="s">
@@ -10618,7 +10647,7 @@
       <c r="C303" s="20" t="s">
         <v>673</v>
       </c>
-      <c r="D303" s="18" t="s">
+      <c r="D303" s="60" t="s">
         <v>820</v>
       </c>
       <c r="E303" s="19" t="s">
@@ -10646,7 +10675,7 @@
       <c r="C304" s="20" t="s">
         <v>674</v>
       </c>
-      <c r="D304" s="18" t="s">
+      <c r="D304" s="60" t="s">
         <v>821</v>
       </c>
       <c r="E304" s="19" t="s">
@@ -10674,7 +10703,7 @@
       <c r="C305" s="20" t="s">
         <v>675</v>
       </c>
-      <c r="D305" s="18" t="s">
+      <c r="D305" s="60" t="s">
         <v>170</v>
       </c>
       <c r="E305" s="19" t="s">
@@ -10702,7 +10731,7 @@
       <c r="C306" s="20" t="s">
         <v>676</v>
       </c>
-      <c r="D306" s="18" t="s">
+      <c r="D306" s="60" t="s">
         <v>171</v>
       </c>
       <c r="E306" s="19" t="s">
@@ -10730,7 +10759,7 @@
       <c r="C307" s="20" t="s">
         <v>677</v>
       </c>
-      <c r="D307" s="18" t="s">
+      <c r="D307" s="60" t="s">
         <v>241</v>
       </c>
       <c r="E307" s="19" t="s">
@@ -10758,7 +10787,7 @@
       <c r="C308" s="20" t="s">
         <v>678</v>
       </c>
-      <c r="D308" s="18" t="s">
+      <c r="D308" s="60" t="s">
         <v>243</v>
       </c>
       <c r="E308" s="19" t="s">
@@ -10786,7 +10815,7 @@
       <c r="C309" s="20" t="s">
         <v>679</v>
       </c>
-      <c r="D309" s="18" t="s">
+      <c r="D309" s="60" t="s">
         <v>272</v>
       </c>
       <c r="E309" s="19" t="s">
@@ -10814,10 +10843,10 @@
       <c r="C310" s="20" t="s">
         <v>680</v>
       </c>
-      <c r="D310" s="18" t="s">
+      <c r="D310" s="60" t="s">
         <v>172</v>
       </c>
-      <c r="E310" s="51" t="s">
+      <c r="E310" s="50" t="s">
         <v>28</v>
       </c>
       <c r="F310" s="24">
@@ -10845,7 +10874,7 @@
       <c r="D311" s="18" t="s">
         <v>327</v>
       </c>
-      <c r="E311" s="51" t="s">
+      <c r="E311" s="50" t="s">
         <v>28</v>
       </c>
       <c r="F311" s="24">
@@ -10873,7 +10902,7 @@
       <c r="D312" s="18" t="s">
         <v>329</v>
       </c>
-      <c r="E312" s="51" t="s">
+      <c r="E312" s="50" t="s">
         <v>28</v>
       </c>
       <c r="F312" s="24">
@@ -10898,10 +10927,10 @@
       <c r="C313" s="20" t="s">
         <v>683</v>
       </c>
-      <c r="D313" s="18" t="s">
+      <c r="D313" s="60" t="s">
         <v>440</v>
       </c>
-      <c r="E313" s="51" t="s">
+      <c r="E313" s="50" t="s">
         <v>28</v>
       </c>
       <c r="F313" s="24">
@@ -10929,7 +10958,7 @@
       <c r="D314" s="18" t="s">
         <v>291</v>
       </c>
-      <c r="E314" s="51" t="s">
+      <c r="E314" s="50" t="s">
         <v>16</v>
       </c>
       <c r="F314" s="24">
@@ -10957,7 +10986,7 @@
       <c r="D315" s="18" t="s">
         <v>342</v>
       </c>
-      <c r="E315" s="51" t="s">
+      <c r="E315" s="50" t="s">
         <v>16</v>
       </c>
       <c r="F315" s="24">
@@ -11264,7 +11293,7 @@
       <c r="C328" s="20" t="s">
         <v>696</v>
       </c>
-      <c r="D328" s="18" t="s">
+      <c r="D328" s="60" t="s">
         <v>182</v>
       </c>
       <c r="E328" s="19" t="s">
@@ -11320,7 +11349,7 @@
       <c r="C330" s="20" t="s">
         <v>698</v>
       </c>
-      <c r="D330" s="18" t="s">
+      <c r="D330" s="60" t="s">
         <v>276</v>
       </c>
       <c r="E330" s="19" t="s">
@@ -11348,7 +11377,7 @@
       <c r="C331" s="20" t="s">
         <v>699</v>
       </c>
-      <c r="D331" s="18" t="s">
+      <c r="D331" s="60" t="s">
         <v>183</v>
       </c>
       <c r="E331" s="19" t="s">
@@ -11460,7 +11489,7 @@
       <c r="C335" s="20" t="s">
         <v>830</v>
       </c>
-      <c r="D335" s="18" t="s">
+      <c r="D335" s="60" t="s">
         <v>829</v>
       </c>
       <c r="E335" s="19" t="s">
@@ -11544,7 +11573,7 @@
       <c r="C338" s="20" t="s">
         <v>705</v>
       </c>
-      <c r="D338" s="18" t="s">
+      <c r="D338" s="60" t="s">
         <v>343</v>
       </c>
       <c r="E338" s="19" t="s">
@@ -11558,7 +11587,7 @@
       <c r="C339" s="20" t="s">
         <v>706</v>
       </c>
-      <c r="D339" s="18" t="s">
+      <c r="D339" s="60" t="s">
         <v>449</v>
       </c>
       <c r="E339" s="19" t="s">
@@ -11572,7 +11601,7 @@
       <c r="C340" s="20" t="s">
         <v>707</v>
       </c>
-      <c r="D340" s="18" t="s">
+      <c r="D340" s="60" t="s">
         <v>455</v>
       </c>
       <c r="E340" s="19" t="s">
@@ -11586,7 +11615,7 @@
       <c r="C341" s="20" t="s">
         <v>708</v>
       </c>
-      <c r="D341" s="18" t="s">
+      <c r="D341" s="60" t="s">
         <v>456</v>
       </c>
       <c r="E341" s="19" t="s">
@@ -11624,7 +11653,7 @@
       <c r="C343" s="20" t="s">
         <v>711</v>
       </c>
-      <c r="D343" s="47" t="s">
+      <c r="D343" s="65" t="s">
         <v>277</v>
       </c>
       <c r="E343" s="19" t="s">
@@ -11638,7 +11667,7 @@
       <c r="C344" s="20" t="s">
         <v>712</v>
       </c>
-      <c r="D344" s="47" t="s">
+      <c r="D344" s="65" t="s">
         <v>278</v>
       </c>
       <c r="E344" s="19" t="s">
@@ -11652,7 +11681,7 @@
       <c r="C345" s="20" t="s">
         <v>713</v>
       </c>
-      <c r="D345" s="47" t="s">
+      <c r="D345" s="65" t="s">
         <v>833</v>
       </c>
       <c r="E345" s="19" t="s">
@@ -11690,7 +11719,7 @@
       <c r="C347" s="20" t="s">
         <v>714</v>
       </c>
-      <c r="D347" s="27" t="s">
+      <c r="D347" s="62" t="s">
         <v>834</v>
       </c>
       <c r="E347" s="40" t="s">
@@ -11704,7 +11733,7 @@
       <c r="C348" s="20" t="s">
         <v>715</v>
       </c>
-      <c r="D348" s="52" t="s">
+      <c r="D348" s="51" t="s">
         <v>835</v>
       </c>
       <c r="E348" s="19" t="s">
@@ -11718,7 +11747,7 @@
       <c r="C349" s="20" t="s">
         <v>709</v>
       </c>
-      <c r="D349" s="52" t="s">
+      <c r="D349" s="51" t="s">
         <v>308</v>
       </c>
       <c r="E349" s="19" t="s">
@@ -11732,7 +11761,7 @@
       <c r="C350" s="20" t="s">
         <v>716</v>
       </c>
-      <c r="D350" s="52" t="s">
+      <c r="D350" s="51" t="s">
         <v>836</v>
       </c>
       <c r="E350" s="19" t="s">
@@ -11746,7 +11775,7 @@
       <c r="C351" s="20" t="s">
         <v>717</v>
       </c>
-      <c r="D351" s="52" t="s">
+      <c r="D351" s="66" t="s">
         <v>447</v>
       </c>
       <c r="E351" s="19" t="s">
@@ -11760,7 +11789,7 @@
       <c r="C352" s="20" t="s">
         <v>718</v>
       </c>
-      <c r="D352" s="52" t="s">
+      <c r="D352" s="66" t="s">
         <v>280</v>
       </c>
       <c r="E352" s="19" t="s">
@@ -11774,7 +11803,7 @@
       <c r="C353" s="20" t="s">
         <v>719</v>
       </c>
-      <c r="D353" s="27" t="s">
+      <c r="D353" s="62" t="s">
         <v>279</v>
       </c>
       <c r="E353" s="19" t="s">
@@ -11788,7 +11817,7 @@
       <c r="C354" s="20" t="s">
         <v>720</v>
       </c>
-      <c r="D354" s="27" t="s">
+      <c r="D354" s="62" t="s">
         <v>837</v>
       </c>
       <c r="E354" s="19" t="s">
@@ -11816,7 +11845,7 @@
       <c r="C356" s="20" t="s">
         <v>722</v>
       </c>
-      <c r="D356" s="27" t="s">
+      <c r="D356" s="62" t="s">
         <v>444</v>
       </c>
       <c r="E356" s="19" t="s">
@@ -11872,7 +11901,7 @@
       <c r="C358" s="20" t="s">
         <v>724</v>
       </c>
-      <c r="D358" s="52" t="s">
+      <c r="D358" s="66" t="s">
         <v>186</v>
       </c>
       <c r="E358" s="19" t="s">
@@ -11900,7 +11929,7 @@
       <c r="C359" s="20" t="s">
         <v>725</v>
       </c>
-      <c r="D359" s="52" t="s">
+      <c r="D359" s="66" t="s">
         <v>809</v>
       </c>
       <c r="E359" s="19" t="s">
@@ -11928,7 +11957,7 @@
       <c r="C360" s="20" t="s">
         <v>726</v>
       </c>
-      <c r="D360" s="52" t="s">
+      <c r="D360" s="51" t="s">
         <v>187</v>
       </c>
       <c r="E360" s="19" t="s">
@@ -11956,7 +11985,7 @@
       <c r="C361" s="20" t="s">
         <v>727</v>
       </c>
-      <c r="D361" s="52" t="s">
+      <c r="D361" s="51" t="s">
         <v>188</v>
       </c>
       <c r="E361" s="19" t="s">
@@ -11984,7 +12013,7 @@
       <c r="C362" s="20" t="s">
         <v>728</v>
       </c>
-      <c r="D362" s="52" t="s">
+      <c r="D362" s="51" t="s">
         <v>813</v>
       </c>
       <c r="E362" s="19" t="s">
@@ -12012,7 +12041,7 @@
       <c r="C363" s="20" t="s">
         <v>729</v>
       </c>
-      <c r="D363" s="52" t="s">
+      <c r="D363" s="66" t="s">
         <v>812</v>
       </c>
       <c r="E363" s="19" t="s">
@@ -12040,7 +12069,7 @@
       <c r="C364" s="20" t="s">
         <v>730</v>
       </c>
-      <c r="D364" s="52" t="s">
+      <c r="D364" s="51" t="s">
         <v>810</v>
       </c>
       <c r="E364" s="19" t="s">
@@ -12068,7 +12097,7 @@
       <c r="C365" s="20" t="s">
         <v>731</v>
       </c>
-      <c r="D365" s="52" t="s">
+      <c r="D365" s="51" t="s">
         <v>446</v>
       </c>
       <c r="E365" s="19" t="s">
@@ -12096,7 +12125,7 @@
       <c r="C366" s="20" t="s">
         <v>732</v>
       </c>
-      <c r="D366" s="52" t="s">
+      <c r="D366" s="51" t="s">
         <v>811</v>
       </c>
       <c r="E366" s="19" t="s">
@@ -12124,7 +12153,7 @@
       <c r="C367" s="20" t="s">
         <v>733</v>
       </c>
-      <c r="D367" s="52" t="s">
+      <c r="D367" s="51" t="s">
         <v>267</v>
       </c>
       <c r="E367" s="19" t="s">
@@ -12152,7 +12181,7 @@
       <c r="C368" s="20" t="s">
         <v>734</v>
       </c>
-      <c r="D368" s="52" t="s">
+      <c r="D368" s="66" t="s">
         <v>189</v>
       </c>
       <c r="E368" s="19" t="s">
@@ -12180,10 +12209,10 @@
       <c r="C369" s="20" t="s">
         <v>735</v>
       </c>
-      <c r="D369" s="18" t="s">
+      <c r="D369" s="60" t="s">
         <v>281</v>
       </c>
-      <c r="E369" s="53" t="s">
+      <c r="E369" s="52" t="s">
         <v>8</v>
       </c>
       <c r="F369" s="19">
@@ -12232,7 +12261,7 @@
       <c r="C371" s="20" t="s">
         <v>736</v>
       </c>
-      <c r="D371" s="18" t="s">
+      <c r="D371" s="60" t="s">
         <v>428</v>
       </c>
       <c r="E371" s="19" t="s">
@@ -12260,7 +12289,7 @@
       <c r="C372" s="20" t="s">
         <v>737</v>
       </c>
-      <c r="D372" s="18" t="s">
+      <c r="D372" s="60" t="s">
         <v>429</v>
       </c>
       <c r="E372" s="19" t="s">
@@ -12288,7 +12317,7 @@
       <c r="C373" s="20" t="s">
         <v>738</v>
       </c>
-      <c r="D373" s="18" t="s">
+      <c r="D373" s="60" t="s">
         <v>191</v>
       </c>
       <c r="E373" s="40" t="s">
@@ -12316,7 +12345,7 @@
       <c r="C374" s="20" t="s">
         <v>739</v>
       </c>
-      <c r="D374" s="18" t="s">
+      <c r="D374" s="60" t="s">
         <v>316</v>
       </c>
       <c r="E374" s="40" t="s">
@@ -12344,7 +12373,7 @@
       <c r="C375" s="20" t="s">
         <v>740</v>
       </c>
-      <c r="D375" s="18" t="s">
+      <c r="D375" s="60" t="s">
         <v>320</v>
       </c>
       <c r="E375" s="40" t="s">
@@ -12372,11 +12401,11 @@
       <c r="C376" s="36">
         <v>14</v>
       </c>
-      <c r="D376" s="54" t="s">
+      <c r="D376" s="53" t="s">
         <v>192</v>
       </c>
-      <c r="E376" s="55"/>
-      <c r="F376" s="55"/>
+      <c r="E376" s="54"/>
+      <c r="F376" s="54"/>
       <c r="G376" s="15"/>
       <c r="H376" s="15"/>
       <c r="I376" s="15"/>
@@ -12396,13 +12425,13 @@
       <c r="C377" s="17" t="s">
         <v>741</v>
       </c>
-      <c r="D377" s="18" t="s">
+      <c r="D377" s="60" t="s">
         <v>193</v>
       </c>
-      <c r="E377" s="48" t="s">
+      <c r="E377" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="F377" s="48">
+      <c r="F377" s="47">
         <v>1</v>
       </c>
       <c r="G377" s="41"/>
@@ -12424,13 +12453,13 @@
       <c r="C378" s="17" t="s">
         <v>742</v>
       </c>
-      <c r="D378" s="18" t="s">
+      <c r="D378" s="60" t="s">
         <v>194</v>
       </c>
       <c r="E378" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="F378" s="56">
+      <c r="F378" s="55">
         <v>1</v>
       </c>
       <c r="G378" s="41"/>
@@ -12455,10 +12484,10 @@
       <c r="D379" s="18" t="s">
         <v>195</v>
       </c>
-      <c r="E379" s="48" t="s">
+      <c r="E379" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="F379" s="57">
+      <c r="F379" s="56">
         <v>1</v>
       </c>
     </row>
@@ -12472,7 +12501,7 @@
       <c r="E380" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="F380" s="56">
+      <c r="F380" s="55">
         <v>1</v>
       </c>
     </row>
@@ -12486,7 +12515,7 @@
       <c r="E381" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="F381" s="56">
+      <c r="F381" s="55">
         <v>1</v>
       </c>
       <c r="G381" s="16"/>
@@ -12514,7 +12543,7 @@
       <c r="E382" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="F382" s="56">
+      <c r="F382" s="55">
         <v>1</v>
       </c>
       <c r="G382" s="16"/>
@@ -12542,7 +12571,7 @@
       <c r="E383" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="F383" s="56">
+      <c r="F383" s="55">
         <v>1</v>
       </c>
       <c r="G383" s="16"/>
@@ -12570,7 +12599,7 @@
       <c r="E384" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="F384" s="56">
+      <c r="F384" s="55">
         <v>1</v>
       </c>
       <c r="G384" s="41"/>
@@ -12598,7 +12627,7 @@
       <c r="E385" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="F385" s="56">
+      <c r="F385" s="55">
         <v>1</v>
       </c>
     </row>
@@ -12620,13 +12649,13 @@
       <c r="C387" s="17" t="s">
         <v>751</v>
       </c>
-      <c r="D387" s="18" t="s">
+      <c r="D387" s="60" t="s">
         <v>201</v>
       </c>
       <c r="E387" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="F387" s="56">
+      <c r="F387" s="55">
         <v>1</v>
       </c>
     </row>
@@ -12634,13 +12663,13 @@
       <c r="C388" s="17" t="s">
         <v>752</v>
       </c>
-      <c r="D388" s="18" t="s">
+      <c r="D388" s="60" t="s">
         <v>202</v>
       </c>
       <c r="E388" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="F388" s="56">
+      <c r="F388" s="55">
         <v>1</v>
       </c>
     </row>
@@ -12654,7 +12683,7 @@
       <c r="E389" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="F389" s="56">
+      <c r="F389" s="55">
         <v>1</v>
       </c>
     </row>
@@ -12668,7 +12697,7 @@
       <c r="E390" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="F390" s="56">
+      <c r="F390" s="55">
         <v>1</v>
       </c>
     </row>
@@ -12676,13 +12705,13 @@
       <c r="C391" s="17" t="s">
         <v>755</v>
       </c>
-      <c r="D391" s="18" t="s">
+      <c r="D391" s="60" t="s">
         <v>205</v>
       </c>
       <c r="E391" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="F391" s="56">
+      <c r="F391" s="55">
         <v>1</v>
       </c>
     </row>
@@ -12696,7 +12725,7 @@
       <c r="E392" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="F392" s="56">
+      <c r="F392" s="55">
         <v>1</v>
       </c>
     </row>
@@ -12704,11 +12733,11 @@
       <c r="C393" s="36">
         <v>15</v>
       </c>
-      <c r="D393" s="54" t="s">
+      <c r="D393" s="53" t="s">
         <v>207</v>
       </c>
-      <c r="E393" s="55"/>
-      <c r="F393" s="55"/>
+      <c r="E393" s="54"/>
+      <c r="F393" s="54"/>
       <c r="G393" s="15"/>
       <c r="H393" s="15"/>
       <c r="I393" s="15"/>
@@ -12728,7 +12757,7 @@
       <c r="C394" s="20" t="s">
         <v>757</v>
       </c>
-      <c r="D394" s="18" t="s">
+      <c r="D394" s="60" t="s">
         <v>208</v>
       </c>
       <c r="E394" s="19" t="s">
@@ -12756,13 +12785,13 @@
       <c r="C395" s="20" t="s">
         <v>758</v>
       </c>
-      <c r="D395" s="18" t="s">
+      <c r="D395" s="60" t="s">
         <v>209</v>
       </c>
       <c r="E395" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="F395" s="56">
+      <c r="F395" s="55">
         <v>1</v>
       </c>
       <c r="G395" s="41"/>
@@ -12784,7 +12813,7 @@
       <c r="C396" s="20" t="s">
         <v>759</v>
       </c>
-      <c r="D396" s="18" t="s">
+      <c r="D396" s="60" t="s">
         <v>210</v>
       </c>
       <c r="E396" s="19" t="s">
@@ -12812,7 +12841,7 @@
       <c r="C397" s="20" t="s">
         <v>760</v>
       </c>
-      <c r="D397" s="18" t="s">
+      <c r="D397" s="60" t="s">
         <v>453</v>
       </c>
       <c r="E397" s="19" t="s">
@@ -12840,7 +12869,7 @@
       <c r="C398" s="20" t="s">
         <v>761</v>
       </c>
-      <c r="D398" s="18" t="s">
+      <c r="D398" s="60" t="s">
         <v>211</v>
       </c>
       <c r="E398" s="19" t="s">
@@ -12868,7 +12897,7 @@
       <c r="C399" s="20" t="s">
         <v>762</v>
       </c>
-      <c r="D399" s="18" t="s">
+      <c r="D399" s="60" t="s">
         <v>454</v>
       </c>
       <c r="E399" s="19" t="s">
@@ -12896,7 +12925,7 @@
       <c r="C400" s="20" t="s">
         <v>763</v>
       </c>
-      <c r="D400" s="18" t="s">
+      <c r="D400" s="60" t="s">
         <v>282</v>
       </c>
       <c r="E400" s="19" t="s">
@@ -12924,7 +12953,7 @@
       <c r="C401" s="20" t="s">
         <v>764</v>
       </c>
-      <c r="D401" s="18" t="s">
+      <c r="D401" s="60" t="s">
         <v>448</v>
       </c>
       <c r="E401" s="19" t="s">
@@ -13004,7 +13033,7 @@
       <c r="C404" s="20" t="s">
         <v>766</v>
       </c>
-      <c r="D404" s="27" t="s">
+      <c r="D404" s="62" t="s">
         <v>296</v>
       </c>
       <c r="E404" s="19" t="s">
@@ -13030,7 +13059,7 @@
       <c r="C405" s="20" t="s">
         <v>767</v>
       </c>
-      <c r="D405" s="18" t="s">
+      <c r="D405" s="60" t="s">
         <v>297</v>
       </c>
       <c r="E405" s="19" t="s">
@@ -13058,7 +13087,7 @@
       <c r="C406" s="20" t="s">
         <v>768</v>
       </c>
-      <c r="D406" s="18" t="s">
+      <c r="D406" s="60" t="s">
         <v>213</v>
       </c>
       <c r="E406" s="40" t="s">
@@ -13086,7 +13115,7 @@
       <c r="C407" s="20" t="s">
         <v>769</v>
       </c>
-      <c r="D407" s="18" t="s">
+      <c r="D407" s="60" t="s">
         <v>214</v>
       </c>
       <c r="E407" s="19" t="s">
@@ -13170,11 +13199,11 @@
       <c r="C410" s="36">
         <v>17</v>
       </c>
-      <c r="D410" s="54" t="s">
+      <c r="D410" s="53" t="s">
         <v>216</v>
       </c>
-      <c r="E410" s="55"/>
-      <c r="F410" s="55"/>
+      <c r="E410" s="54"/>
+      <c r="F410" s="54"/>
       <c r="G410" s="15"/>
       <c r="H410" s="15"/>
       <c r="I410" s="15"/>
@@ -13208,7 +13237,7 @@
       <c r="C412" s="20" t="s">
         <v>773</v>
       </c>
-      <c r="D412" s="18" t="s">
+      <c r="D412" s="60" t="s">
         <v>218</v>
       </c>
       <c r="E412" s="40" t="s">
@@ -13236,7 +13265,7 @@
       <c r="C414" s="20" t="s">
         <v>775</v>
       </c>
-      <c r="D414" s="18" t="s">
+      <c r="D414" s="60" t="s">
         <v>221</v>
       </c>
       <c r="E414" s="19" t="s">
@@ -13250,7 +13279,7 @@
       <c r="C415" s="20" t="s">
         <v>776</v>
       </c>
-      <c r="D415" s="18" t="s">
+      <c r="D415" s="60" t="s">
         <v>222</v>
       </c>
       <c r="E415" s="40" t="s">
@@ -13278,7 +13307,7 @@
       <c r="C416" s="20" t="s">
         <v>777</v>
       </c>
-      <c r="D416" s="18" t="s">
+      <c r="D416" s="60" t="s">
         <v>223</v>
       </c>
       <c r="E416" s="40" t="s">
@@ -13334,7 +13363,7 @@
       <c r="C418" s="20" t="s">
         <v>779</v>
       </c>
-      <c r="D418" s="18" t="s">
+      <c r="D418" s="60" t="s">
         <v>442</v>
       </c>
       <c r="E418" s="19" t="s">
@@ -13362,7 +13391,7 @@
       <c r="C419" s="20" t="s">
         <v>780</v>
       </c>
-      <c r="D419" s="18" t="s">
+      <c r="D419" s="60" t="s">
         <v>225</v>
       </c>
       <c r="E419" s="40" t="s">
@@ -13390,7 +13419,7 @@
       <c r="C420" s="20" t="s">
         <v>781</v>
       </c>
-      <c r="D420" s="18" t="s">
+      <c r="D420" s="60" t="s">
         <v>226</v>
       </c>
       <c r="E420" s="19" t="s">
@@ -13419,7 +13448,7 @@
       <c r="C421" s="20" t="s">
         <v>782</v>
       </c>
-      <c r="D421" s="18" t="s">
+      <c r="D421" s="60" t="s">
         <v>227</v>
       </c>
       <c r="E421" s="40" t="s">
@@ -13448,7 +13477,7 @@
       <c r="C422" s="20" t="s">
         <v>783</v>
       </c>
-      <c r="D422" s="18" t="s">
+      <c r="D422" s="60" t="s">
         <v>228</v>
       </c>
       <c r="E422" s="40" t="s">
@@ -13477,7 +13506,7 @@
       <c r="C423" s="20" t="s">
         <v>784</v>
       </c>
-      <c r="D423" s="18" t="s">
+      <c r="D423" s="60" t="s">
         <v>229</v>
       </c>
       <c r="E423" s="40" t="s">
@@ -13535,7 +13564,7 @@
       <c r="C425" s="20" t="s">
         <v>786</v>
       </c>
-      <c r="D425" s="18" t="s">
+      <c r="D425" s="60" t="s">
         <v>443</v>
       </c>
       <c r="E425" s="40" t="s">

</xml_diff>